<commit_message>
Fixed bugs in sceneration package, minor updates
Signed-off-by: Aytug Yavuzer <aytug.yavuzer@rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/tutorials/scenariogeneration/input_generator.xlsx
+++ b/tutorials/scenariogeneration/input_generator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aytugy\Desktop\workspace\multi_mg_mgm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABAEB11-AD38-4AB7-980B-A7104720DDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FFE628C-3524-4740-B3AD-754D366DE11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{786279F1-1AC9-41FC-9C31-90F9BBEA2A7F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{786279F1-1AC9-41FC-9C31-90F9BBEA2A7F}"/>
   </bookViews>
   <sheets>
     <sheet name="ArrivalTime" sheetId="1" r:id="rId1"/>
@@ -164,6 +164,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -179,12 +182,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -199,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -208,6 +217,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2361,15 +2372,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB5282A1-D372-415A-B507-3E13FF571B9A}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -2387,264 +2397,264 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>4.1666666666666664E-2</v>
+      <c r="B2" s="4">
+        <v>44348.291666666664</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44348.333333333336</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>4.1666666666666699E-2</v>
-      </c>
-      <c r="C3" s="3">
-        <v>8.3333333333333301E-2</v>
+      <c r="B3" s="4">
+        <v>44348.333333333336</v>
+      </c>
+      <c r="C3" s="4">
+        <v>44348.375000057873</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>8.3333333333333301E-2</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0.125</v>
+      <c r="B4" s="4">
+        <v>44348.375000057873</v>
+      </c>
+      <c r="C4" s="4">
+        <v>44348.41666678241</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.125</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.16666666666666699</v>
+      <c r="B5" s="4">
+        <v>44348.41666678241</v>
+      </c>
+      <c r="C5" s="4">
+        <v>44348.458333506947</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.16666666666666699</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0.20833333333333301</v>
+      <c r="B6" s="4">
+        <v>44348.458333506947</v>
+      </c>
+      <c r="C6" s="4">
+        <v>44348.500000231485</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.20833333333333301</v>
-      </c>
-      <c r="C7" s="3">
-        <v>0.25</v>
+      <c r="B7" s="4">
+        <v>44348.500000231485</v>
+      </c>
+      <c r="C7" s="4">
+        <v>44348.541666956022</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0.29166666666666702</v>
+      <c r="B8" s="4">
+        <v>44348.541666956022</v>
+      </c>
+      <c r="C8" s="4">
+        <v>44348.583333680559</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.29166666666666702</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.33333333333333298</v>
+      <c r="B9" s="4">
+        <v>44348.583333680559</v>
+      </c>
+      <c r="C9" s="4">
+        <v>44348.625000405096</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.33333333333333298</v>
-      </c>
-      <c r="C10" s="3">
-        <v>0.375</v>
+      <c r="B10" s="4">
+        <v>44348.625000405096</v>
+      </c>
+      <c r="C10" s="4">
+        <v>44348.666667129626</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.375</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.41666666666666702</v>
+      <c r="B11" s="4">
+        <v>44348.666667129626</v>
+      </c>
+      <c r="C11" s="4">
+        <v>44348.708333854163</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="2">
-        <v>0.41666666666666702</v>
-      </c>
-      <c r="C12" s="3">
-        <v>0.45833333333333298</v>
+      <c r="B12" s="4">
+        <v>44348.708333854163</v>
+      </c>
+      <c r="C12" s="4">
+        <v>44348.750000578701</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="2">
-        <v>0.45833333333333298</v>
-      </c>
-      <c r="C13" s="3">
-        <v>0.5</v>
+      <c r="B13" s="4">
+        <v>44348.750000578701</v>
+      </c>
+      <c r="C13" s="4">
+        <v>44348.791667303238</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.54166666666666696</v>
+      <c r="B14" s="4">
+        <v>44348.791667303238</v>
+      </c>
+      <c r="C14" s="4">
+        <v>44348.833334027775</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="C15" s="3">
-        <v>0.58333333333333304</v>
+      <c r="B15" s="4">
+        <v>44348.833334027775</v>
+      </c>
+      <c r="C15" s="4">
+        <v>44348.875000752312</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.625</v>
+      <c r="B16" s="4">
+        <v>44348.875000752312</v>
+      </c>
+      <c r="C16" s="4">
+        <v>44348.916667476849</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
-        <v>0.625</v>
-      </c>
-      <c r="C17" s="3">
-        <v>0.66666666666666696</v>
+      <c r="B17" s="4">
+        <v>44348.916667476849</v>
+      </c>
+      <c r="C17" s="4">
+        <v>44348.958334201387</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="2">
-        <v>0.66666666666666696</v>
-      </c>
-      <c r="C18" s="3">
-        <v>0.70833333333333304</v>
+      <c r="B18" s="4">
+        <v>44348.958334201387</v>
+      </c>
+      <c r="C18" s="4">
+        <v>44349.000000925924</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="2">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="C19" s="3">
-        <v>0.75</v>
+      <c r="B19" s="4">
+        <v>44349.000000925924</v>
+      </c>
+      <c r="C19" s="4">
+        <v>44349.041667650461</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.79166666666666696</v>
+      <c r="B20" s="4">
+        <v>44349.041667650461</v>
+      </c>
+      <c r="C20" s="4">
+        <v>44349.083334374998</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="2">
-        <v>0.79166666666666696</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0.83333333333333304</v>
+      <c r="B21" s="4">
+        <v>44349.083334374998</v>
+      </c>
+      <c r="C21" s="4">
+        <v>44349.125001099535</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="2">
-        <v>0.83333333333333304</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0.875</v>
+      <c r="B22" s="4">
+        <v>44349.125001099535</v>
+      </c>
+      <c r="C22" s="4">
+        <v>44349.166667824073</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
-        <v>0.875</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0.91666666666666696</v>
+      <c r="B23" s="4">
+        <v>44349.166667824073</v>
+      </c>
+      <c r="C23" s="4">
+        <v>44349.20833454861</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="2">
-        <v>0.91666666666666696</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0.95833333333333304</v>
+      <c r="B24" s="4">
+        <v>44349.20833454861</v>
+      </c>
+      <c r="C24" s="4">
+        <v>44349.250001273147</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="2">
-        <v>0.95833333333333304</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0</v>
+      <c r="B25" s="4">
+        <v>44349.250001273147</v>
+      </c>
+      <c r="C25" s="4">
+        <v>44349.291667939811</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -5231,8 +5241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFEAC849-9A27-4C43-88BA-A423954EB3D0}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5240,7 +5250,7 @@
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5254,7 +5264,7 @@
       <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
@@ -5271,7 +5281,7 @@
       <c r="C2">
         <v>6.6</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>56</v>
       </c>
       <c r="E2">
@@ -5288,7 +5298,7 @@
       <c r="C3">
         <v>11</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="5">
         <v>250</v>
       </c>
       <c r="E3">
@@ -5305,7 +5315,7 @@
       <c r="C4">
         <v>11</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="5">
         <v>170</v>
       </c>
       <c r="E4">
@@ -5322,7 +5332,7 @@
       <c r="C5">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="5">
         <v>250</v>
       </c>
       <c r="E5">
@@ -5339,7 +5349,7 @@
       <c r="C6">
         <v>11</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="5">
         <v>200</v>
       </c>
       <c r="E6">
@@ -5356,7 +5366,7 @@
       <c r="C7">
         <v>11</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="5">
         <v>207</v>
       </c>
       <c r="E7">
@@ -5373,7 +5383,7 @@
       <c r="C8">
         <v>11</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="5">
         <v>233</v>
       </c>
       <c r="E8">
@@ -5390,7 +5400,7 @@
       <c r="C9">
         <v>22</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="5">
         <v>130</v>
       </c>
       <c r="E9">
@@ -5407,7 +5417,7 @@
       <c r="C10">
         <v>7.4</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="5">
         <v>130</v>
       </c>
       <c r="E10">
@@ -5424,7 +5434,7 @@
       <c r="C11">
         <v>11</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="5">
         <v>80</v>
       </c>
       <c r="E11">
@@ -5441,7 +5451,7 @@
       <c r="C12">
         <v>11</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>135</v>
       </c>
       <c r="E12">
@@ -5458,7 +5468,7 @@
       <c r="C13">
         <v>11</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="5">
         <v>170</v>
       </c>
       <c r="E13">
@@ -5475,7 +5485,7 @@
       <c r="C14">
         <v>11</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="5">
         <v>196</v>
       </c>
       <c r="E14">
@@ -5492,7 +5502,7 @@
       <c r="C15">
         <v>11</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="5">
         <v>77</v>
       </c>
       <c r="E15">
@@ -5509,7 +5519,7 @@
       <c r="C16">
         <v>11</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="5">
         <v>149</v>
       </c>
       <c r="E16">
@@ -5526,7 +5536,7 @@
       <c r="C17">
         <v>11</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="5">
         <v>233</v>
       </c>
       <c r="E17">
@@ -5543,7 +5553,7 @@
       <c r="C18">
         <v>16.5</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="5">
         <v>250</v>
       </c>
       <c r="E18">
@@ -5560,7 +5570,7 @@
       <c r="C19">
         <v>11</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="5">
         <v>207</v>
       </c>
       <c r="E19">
@@ -5577,7 +5587,7 @@
       <c r="C20">
         <v>11</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="5">
         <v>200</v>
       </c>
       <c r="E20">
@@ -5594,7 +5604,7 @@
       <c r="C21">
         <v>11</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="5">
         <v>265</v>
       </c>
       <c r="E21">

</xml_diff>